<commit_message>
Edit dashboard and setting code
</commit_message>
<xml_diff>
--- a/reference_data/plant_standards_cleaned.xlsx
+++ b/reference_data/plant_standards_cleaned.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\GreenEye_Backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\2025ESW\GreenEye_Backend\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF2773-3DE7-488B-A2D8-EC728A084DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42FFE59-B2C3-4720-8169-184E2EF562A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,9 +352,6 @@
     <t>20 ~ 60</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>22.0</t>
   </si>
   <si>
@@ -376,12 +373,6 @@
     <t>영산홍/철쭉 (Royal Azalea)</t>
   </si>
   <si>
-    <t>5 ~35</t>
-  </si>
-  <si>
-    <t>2200</t>
-  </si>
-  <si>
     <t>22 ~ 26</t>
   </si>
   <si>
@@ -559,9 +550,6 @@
     <t>25000 ~ 50000</t>
   </si>
   <si>
-    <t>10~30</t>
-  </si>
-  <si>
     <t>800 ~ 1500</t>
   </si>
   <si>
@@ -574,12 +562,6 @@
     <t>19 ~ 27</t>
   </si>
   <si>
-    <t>18~24</t>
-  </si>
-  <si>
-    <t>30~40</t>
-  </si>
-  <si>
     <t>400 ~ 1500</t>
   </si>
   <si>
@@ -589,12 +571,6 @@
     <t>에케베리아 (Echeveria)</t>
   </si>
   <si>
-    <t>16~24</t>
-  </si>
-  <si>
-    <t>20~40</t>
-  </si>
-  <si>
     <t>800 ~ 1600</t>
   </si>
   <si>
@@ -607,15 +583,6 @@
     <t>15 ~ 26</t>
   </si>
   <si>
-    <t>7000~15000</t>
-  </si>
-  <si>
-    <t>15~24</t>
-  </si>
-  <si>
-    <t>30~50</t>
-  </si>
-  <si>
     <t>1000 ~ 1800</t>
   </si>
   <si>
@@ -628,15 +595,6 @@
     <t>15 ~ 33</t>
   </si>
   <si>
-    <t>18000~30000</t>
-  </si>
-  <si>
-    <t>15~20</t>
-  </si>
-  <si>
-    <t>40~60</t>
-  </si>
-  <si>
     <t>1000 ~ 2000</t>
   </si>
   <si>
@@ -649,18 +607,6 @@
     <t>18 ~ 26</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>3600~12000</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>50~60</t>
-  </si>
-  <si>
     <t>44.0</t>
   </si>
   <si>
@@ -673,15 +619,6 @@
     <t>70 ~ 75</t>
   </si>
   <si>
-    <t>8000~15000</t>
-  </si>
-  <si>
-    <t>9~12</t>
-  </si>
-  <si>
-    <t>60~80</t>
-  </si>
-  <si>
     <t>45.0</t>
   </si>
   <si>
@@ -694,12 +631,6 @@
     <t>65 ~ 80</t>
   </si>
   <si>
-    <t>8~12</t>
-  </si>
-  <si>
-    <t>70~85</t>
-  </si>
-  <si>
     <t>1200 ~ 2500</t>
   </si>
   <si>
@@ -715,12 +646,6 @@
     <t>80 ~ 90</t>
   </si>
   <si>
-    <t>9~17</t>
-  </si>
-  <si>
-    <t>75~85</t>
-  </si>
-  <si>
     <t>1000 ~ 2200</t>
   </si>
   <si>
@@ -733,12 +658,6 @@
     <t>5 ~ 17</t>
   </si>
   <si>
-    <t>10000~20000</t>
-  </si>
-  <si>
-    <t>10~16</t>
-  </si>
-  <si>
     <t>1200 ~ 2000</t>
   </si>
   <si>
@@ -748,12 +667,6 @@
     <t>글라디올러스 (Gladiolus)</t>
   </si>
   <si>
-    <t>25000~40000</t>
-  </si>
-  <si>
-    <t>65~80</t>
-  </si>
-  <si>
     <t>1400 ~ 2400</t>
   </si>
   <si>
@@ -763,12 +676,6 @@
     <t>아마릴리스 (Amaryllis)</t>
   </si>
   <si>
-    <t>10000~25000</t>
-  </si>
-  <si>
-    <t>50~70</t>
-  </si>
-  <si>
     <t>50.0</t>
   </si>
   <si>
@@ -778,12 +685,6 @@
     <t>4 ~ 15</t>
   </si>
   <si>
-    <t>8000~20000</t>
-  </si>
-  <si>
-    <t>5~12</t>
-  </si>
-  <si>
     <t>51.0</t>
   </si>
   <si>
@@ -805,12 +706,6 @@
     <t>65 ~ 75</t>
   </si>
   <si>
-    <t>15000~30000</t>
-  </si>
-  <si>
-    <t>17~24</t>
-  </si>
-  <si>
     <t>1800 ~ 2500</t>
   </si>
   <si>
@@ -826,9 +721,6 @@
     <t>70 ~ 90</t>
   </si>
   <si>
-    <t>15000~27000</t>
-  </si>
-  <si>
     <t>54.0</t>
   </si>
   <si>
@@ -841,9 +733,6 @@
     <t>70 ~ 80</t>
   </si>
   <si>
-    <t>9~18</t>
-  </si>
-  <si>
     <t>1400 ~ 2500</t>
   </si>
   <si>
@@ -856,12 +745,6 @@
     <t>65 ~ 85</t>
   </si>
   <si>
-    <t>16~22</t>
-  </si>
-  <si>
-    <t>60~75</t>
-  </si>
-  <si>
     <t>2000 ~ 3500</t>
   </si>
   <si>
@@ -874,12 +757,6 @@
     <t>17 ~ 34</t>
   </si>
   <si>
-    <t>25000~100000</t>
-  </si>
-  <si>
-    <t>12~20</t>
-  </si>
-  <si>
     <t>500 ~ 2000</t>
   </si>
   <si>
@@ -895,202 +772,362 @@
     <t>810 ~ 2150</t>
   </si>
   <si>
+    <t>58.0</t>
+  </si>
+  <si>
+    <t>아글라오네마 (Aglaonema)</t>
+  </si>
+  <si>
+    <t>45 ~ 60</t>
+  </si>
+  <si>
+    <t>270 ~ 2150</t>
+  </si>
+  <si>
+    <t>59.0</t>
+  </si>
+  <si>
+    <t>디펜바키아 (Dieffenbachia)</t>
+  </si>
+  <si>
+    <t>1600 ~ 2700</t>
+  </si>
+  <si>
+    <t>30 ~ 40</t>
+  </si>
+  <si>
+    <t>1200 ~ 2200</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>몬스테라 (Monstera)</t>
+  </si>
+  <si>
+    <t>800 ~ 10000</t>
+  </si>
+  <si>
+    <t>28 ~ 38</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>산세베리아 (Sansevieria)</t>
+  </si>
+  <si>
+    <t>21 ~ 25</t>
+  </si>
+  <si>
+    <t>270 ~ 4300</t>
+  </si>
+  <si>
+    <t>22 ~ 25</t>
+  </si>
+  <si>
+    <t>12 ~ 22</t>
+  </si>
+  <si>
+    <t>500 ~ 1200</t>
+  </si>
+  <si>
+    <t>62.0</t>
+  </si>
+  <si>
+    <t>테이블야자 (Parlor palm)</t>
+  </si>
+  <si>
+    <t>20 ~ 27</t>
+  </si>
+  <si>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>페페로미아 (Peperomia)</t>
+  </si>
+  <si>
+    <t>25 ~ 35</t>
+  </si>
+  <si>
+    <t>800 ~ 1800</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>벵갈고무나무 (Ficus elastica)</t>
+  </si>
+  <si>
+    <t>810 ~ 4300</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>싱고니움 (Syngonium)</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>칼라디움 (Caladium)</t>
+  </si>
+  <si>
+    <t>35 ~ 45</t>
+  </si>
+  <si>
+    <t>67.0</t>
+  </si>
+  <si>
+    <t>바질 (Basil)</t>
+  </si>
+  <si>
+    <t>20000 ~ 100000</t>
+  </si>
+  <si>
+    <t>30 ~ 45</t>
+  </si>
+  <si>
+    <t>1300 ~ 2000</t>
+  </si>
+  <si>
+    <t>68.0</t>
+  </si>
+  <si>
+    <t>로즈마리 (Rosemary)</t>
+  </si>
+  <si>
+    <t>40 ~ 50</t>
+  </si>
+  <si>
+    <t>69.0</t>
+  </si>
+  <si>
+    <t>타임 / 벼룩이자리 (Thyme)</t>
+  </si>
+  <si>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>오레가노 (Oregano)</t>
+  </si>
+  <si>
+    <t>71.0</t>
+  </si>
+  <si>
+    <t>민트 / 배초향 (Korean Mint)</t>
+  </si>
+  <si>
+    <t>72.0</t>
+  </si>
+  <si>
+    <t>73.0</t>
+  </si>
+  <si>
+    <t>카모마일 / 카밀레 (Chamomile)</t>
+  </si>
+  <si>
+    <t>1000 ~ 1600</t>
+  </si>
+  <si>
+    <t>74.0</t>
+  </si>
+  <si>
+    <t>안개꽃 (Gypsophila)</t>
+  </si>
+  <si>
+    <t>1250 ~ 2000</t>
+  </si>
+  <si>
+    <t>1800 ~ 2200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500 ~ 2500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40 ~ 60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 ~ 25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 ~ 35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 ~ 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 ~ 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 ~ 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 ~ 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 ~ 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7000 ~ 15000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18000 ~ 30000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3600 ~ 12000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000 ~ 15000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000 ~ 20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25000 ~ 40000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000 ~ 25000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000 ~ 20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15000 ~ 30000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15000 ~ 27000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25000 ~ 100000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 ~ 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 ~ 22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 ~ 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 ~ 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 ~ 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 ~ 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 ~ 60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 ~ 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 ~ 85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75 ~ 85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65 ~ 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 ~ 70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 ~ 75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>25 ~ 30</t>
-  </si>
-  <si>
-    <t>58.0</t>
-  </si>
-  <si>
-    <t>아글라오네마 (Aglaonema)</t>
-  </si>
-  <si>
-    <t>45 ~ 60</t>
-  </si>
-  <si>
-    <t>270 ~ 2150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>30 ~ 38</t>
-  </si>
-  <si>
-    <t>59.0</t>
-  </si>
-  <si>
-    <t>디펜바키아 (Dieffenbachia)</t>
-  </si>
-  <si>
-    <t>1600 ~ 2700</t>
-  </si>
-  <si>
-    <t>30 ~ 40</t>
-  </si>
-  <si>
-    <t>1200 ~ 2200</t>
-  </si>
-  <si>
-    <t>60.0</t>
-  </si>
-  <si>
-    <t>몬스테라 (Monstera)</t>
-  </si>
-  <si>
-    <t>800 ~ 10000</t>
-  </si>
-  <si>
-    <t>28 ~ 38</t>
-  </si>
-  <si>
-    <t>61.0</t>
-  </si>
-  <si>
-    <t>산세베리아 (Sansevieria)</t>
-  </si>
-  <si>
-    <t>21 ~ 25</t>
-  </si>
-  <si>
-    <t>270 ~ 4300</t>
-  </si>
-  <si>
-    <t>22 ~ 25</t>
-  </si>
-  <si>
-    <t>12 ~ 22</t>
-  </si>
-  <si>
-    <t>500 ~ 1200</t>
-  </si>
-  <si>
-    <t>62.0</t>
-  </si>
-  <si>
-    <t>테이블야자 (Parlor palm)</t>
-  </si>
-  <si>
-    <t>20 ~ 27</t>
-  </si>
-  <si>
-    <t>63.0</t>
-  </si>
-  <si>
-    <t>페페로미아 (Peperomia)</t>
-  </si>
-  <si>
-    <t>25 ~ 35</t>
-  </si>
-  <si>
-    <t>800 ~ 1800</t>
-  </si>
-  <si>
-    <t>64.0</t>
-  </si>
-  <si>
-    <t>벵갈고무나무 (Ficus elastica)</t>
-  </si>
-  <si>
-    <t>810 ~ 4300</t>
-  </si>
-  <si>
-    <t>65.0</t>
-  </si>
-  <si>
-    <t>싱고니움 (Syngonium)</t>
-  </si>
-  <si>
-    <t>66.0</t>
-  </si>
-  <si>
-    <t>칼라디움 (Caladium)</t>
-  </si>
-  <si>
-    <t>35 ~ 45</t>
-  </si>
-  <si>
-    <t>67.0</t>
-  </si>
-  <si>
-    <t>바질 (Basil)</t>
-  </si>
-  <si>
-    <t>20000 ~ 100000</t>
-  </si>
-  <si>
-    <t>30 ~ 45</t>
-  </si>
-  <si>
-    <t>1300 ~ 2000</t>
-  </si>
-  <si>
-    <t>68.0</t>
-  </si>
-  <si>
-    <t>로즈마리 (Rosemary)</t>
-  </si>
-  <si>
-    <t>40 ~ 50</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
-    <t>타임 / 벼룩이자리 (Thyme)</t>
-  </si>
-  <si>
-    <t>70.0</t>
-  </si>
-  <si>
-    <t>오레가노 (Oregano)</t>
-  </si>
-  <si>
-    <t>71.0</t>
-  </si>
-  <si>
-    <t>민트 / 배초향 (Korean Mint)</t>
-  </si>
-  <si>
-    <t>72.0</t>
-  </si>
-  <si>
-    <t>73.0</t>
-  </si>
-  <si>
-    <t>카모마일 / 카밀레 (Chamomile)</t>
-  </si>
-  <si>
-    <t>1000 ~ 1600</t>
-  </si>
-  <si>
-    <t>74.0</t>
-  </si>
-  <si>
-    <t>안개꽃 (Gypsophila)</t>
-  </si>
-  <si>
-    <t>1250 ~ 2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>환경온도(°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>환경습도(%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>환경광도(lux)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>토양온도(°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>토양수분(%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>토양전도도(uS/cm)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1465,10 +1502,19 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <cols>
+    <col min="2" max="2" width="28.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -2039,15 +2085,15 @@
         <v>109</v>
       </c>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
         <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
       </c>
       <c r="C23" t="s">
         <v>106</v>
@@ -2056,50 +2102,50 @@
         <v>16</v>
       </c>
       <c r="E23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" t="s">
         <v>113</v>
-      </c>
-      <c r="F23" t="s">
-        <v>114</v>
       </c>
       <c r="G23" t="s">
         <v>108</v>
       </c>
       <c r="H23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
         <v>116</v>
       </c>
-      <c r="B24" t="s">
-        <v>117</v>
-      </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>311</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
+        <v>307</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" t="s">
         <v>119</v>
-      </c>
-      <c r="F24" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
         <v>64</v>
@@ -2108,10 +2154,10 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
@@ -2122,45 +2168,45 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
         <v>108</v>
       </c>
       <c r="H26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -2174,22 +2220,22 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" t="s">
         <v>16</v>
@@ -2200,51 +2246,51 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H30" t="s">
         <v>61</v>
@@ -2252,22 +2298,22 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" t="s">
         <v>16</v>
@@ -2278,19 +2324,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F32" t="s">
         <v>108</v>
@@ -2304,10 +2350,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
@@ -2316,85 +2362,85 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F33" t="s">
         <v>36</v>
       </c>
       <c r="G33" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G34" t="s">
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G35" t="s">
         <v>94</v>
       </c>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F36" t="s">
         <v>25</v>
@@ -2403,30 +2449,30 @@
         <v>94</v>
       </c>
       <c r="H36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H37" t="s">
         <v>86</v>
@@ -2434,10 +2480,10 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
@@ -2449,307 +2495,307 @@
         <v>99</v>
       </c>
       <c r="F38" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G38" t="s">
         <v>94</v>
       </c>
       <c r="H38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G39" t="s">
-        <v>179</v>
+        <v>335</v>
       </c>
       <c r="H39" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F40" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="G40" t="s">
-        <v>185</v>
+        <v>336</v>
       </c>
       <c r="H40" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C41" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F41" t="s">
-        <v>189</v>
+        <v>319</v>
       </c>
       <c r="G41" t="s">
-        <v>190</v>
+        <v>337</v>
       </c>
       <c r="H41" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>195</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="G42" t="s">
-        <v>197</v>
+        <v>338</v>
       </c>
       <c r="H42" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B43" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
+        <v>321</v>
       </c>
       <c r="F43" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="G43" t="s">
-        <v>204</v>
+        <v>309</v>
       </c>
       <c r="H43" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B44" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>209</v>
+        <v>309</v>
       </c>
       <c r="E44" t="s">
-        <v>210</v>
+        <v>322</v>
       </c>
       <c r="F44" t="s">
-        <v>211</v>
+        <v>310</v>
       </c>
       <c r="G44" t="s">
-        <v>212</v>
+        <v>339</v>
       </c>
       <c r="H44" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C45" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="D45" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="F45" t="s">
-        <v>218</v>
+        <v>312</v>
       </c>
       <c r="G45" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H45" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="C46" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="E46" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="F46" t="s">
-        <v>224</v>
+        <v>313</v>
       </c>
       <c r="G46" t="s">
-        <v>225</v>
+        <v>341</v>
       </c>
       <c r="H46" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="B47" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="C47" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E47" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="F47" t="s">
-        <v>231</v>
+        <v>314</v>
       </c>
       <c r="G47" t="s">
-        <v>232</v>
+        <v>342</v>
       </c>
       <c r="H47" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="B48" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="C48" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E48" t="s">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="F48" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="G48" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H48" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>308</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E49" t="s">
-        <v>242</v>
+        <v>325</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="G49" t="s">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="H49" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
         <v>64</v>
@@ -2758,258 +2804,258 @@
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>247</v>
+        <v>326</v>
       </c>
       <c r="F50" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="G50" t="s">
-        <v>248</v>
+        <v>345</v>
       </c>
       <c r="H50" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="C51" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="D51" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="E51" t="s">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="F51" t="s">
-        <v>253</v>
+        <v>317</v>
       </c>
       <c r="G51" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H51" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="C52" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D52" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="E52" t="s">
-        <v>242</v>
+        <v>325</v>
       </c>
       <c r="F52" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="G52" t="s">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="H52" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="E53" t="s">
-        <v>261</v>
+        <v>328</v>
       </c>
       <c r="F53" t="s">
-        <v>262</v>
+        <v>333</v>
       </c>
       <c r="G53" t="s">
-        <v>225</v>
+        <v>341</v>
       </c>
       <c r="H53" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D54" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="E54" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
       <c r="F54" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="G54" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H54" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="C55" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="E55" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
       <c r="F55" t="s">
-        <v>273</v>
+        <v>334</v>
       </c>
       <c r="G55" t="s">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="H55" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
       <c r="B56" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
       <c r="C56" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D56" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
       <c r="E56" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
       <c r="F56" t="s">
-        <v>278</v>
+        <v>332</v>
       </c>
       <c r="G56" t="s">
-        <v>279</v>
+        <v>346</v>
       </c>
       <c r="H56" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>281</v>
+        <v>242</v>
       </c>
       <c r="B57" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="C57" t="s">
-        <v>283</v>
+        <v>244</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>284</v>
+        <v>330</v>
       </c>
       <c r="F57" t="s">
-        <v>285</v>
+        <v>331</v>
       </c>
       <c r="G57" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H57" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="B58" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
       <c r="C58" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="D58" t="s">
         <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="F58" t="s">
         <v>36</v>
       </c>
       <c r="G58" t="s">
-        <v>291</v>
+        <v>347</v>
       </c>
       <c r="H58" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>292</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="C59" t="s">
         <v>108</v>
       </c>
       <c r="D59" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="E59" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="F59" t="s">
         <v>108</v>
       </c>
       <c r="G59" t="s">
-        <v>296</v>
+        <v>348</v>
       </c>
       <c r="H59" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B60" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
@@ -3018,24 +3064,24 @@
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="F60" t="s">
         <v>108</v>
       </c>
       <c r="G60" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H60" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C61" t="s">
         <v>25</v>
@@ -3044,76 +3090,76 @@
         <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>304</v>
+        <v>261</v>
       </c>
       <c r="F61" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G61" t="s">
-        <v>305</v>
+        <v>262</v>
       </c>
       <c r="H61" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="C62" t="s">
-        <v>308</v>
+        <v>265</v>
       </c>
       <c r="D62" t="s">
         <v>16</v>
       </c>
       <c r="E62" t="s">
-        <v>309</v>
+        <v>266</v>
       </c>
       <c r="F62" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G62" t="s">
-        <v>311</v>
+        <v>268</v>
       </c>
       <c r="H62" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="B63" t="s">
-        <v>314</v>
+        <v>271</v>
       </c>
       <c r="C63" t="s">
-        <v>315</v>
+        <v>272</v>
       </c>
       <c r="D63" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="E63" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="F63" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G63" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H63" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>316</v>
+        <v>273</v>
       </c>
       <c r="B64" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="C64" t="s">
         <v>36</v>
@@ -3122,180 +3168,180 @@
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="F64" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G64" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H64" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>320</v>
+        <v>277</v>
       </c>
       <c r="B65" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="C65" t="s">
         <v>36</v>
       </c>
       <c r="D65" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="E65" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="F65" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G65" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H65" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>323</v>
+        <v>280</v>
       </c>
       <c r="B66" t="s">
-        <v>324</v>
+        <v>281</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="F66" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G66" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H66" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>325</v>
+        <v>282</v>
       </c>
       <c r="B67" t="s">
-        <v>326</v>
+        <v>283</v>
       </c>
       <c r="C67" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D67" t="s">
         <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="F67" t="s">
         <v>48</v>
       </c>
       <c r="G67" t="s">
-        <v>327</v>
+        <v>284</v>
       </c>
       <c r="H67" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="B68" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F68" t="s">
         <v>65</v>
       </c>
       <c r="G68" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="H68" t="s">
-        <v>332</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>333</v>
+        <v>290</v>
       </c>
       <c r="B69" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
       </c>
       <c r="D69" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E69" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F69" t="s">
         <v>65</v>
       </c>
       <c r="G69" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H69" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="B70" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="C70" t="s">
         <v>15</v>
       </c>
       <c r="D70" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E70" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F70" t="s">
         <v>65</v>
       </c>
       <c r="G70" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H70" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
       <c r="B71" t="s">
-        <v>339</v>
+        <v>296</v>
       </c>
       <c r="C71" t="s">
         <v>15</v>
@@ -3304,47 +3350,47 @@
         <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F71" t="s">
         <v>65</v>
       </c>
       <c r="G71" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H71" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>340</v>
+        <v>297</v>
       </c>
       <c r="B72" t="s">
-        <v>341</v>
+        <v>298</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F72" t="s">
         <v>65</v>
       </c>
       <c r="G72" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H72" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
@@ -3356,68 +3402,68 @@
         <v>19</v>
       </c>
       <c r="E73" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F73" t="s">
         <v>65</v>
       </c>
       <c r="G73" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H73" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>343</v>
+        <v>300</v>
       </c>
       <c r="B74" t="s">
-        <v>344</v>
+        <v>301</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D74" t="s">
         <v>5</v>
       </c>
       <c r="E74" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F74" t="s">
         <v>65</v>
       </c>
       <c r="G74" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H74" t="s">
-        <v>345</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>346</v>
+        <v>303</v>
       </c>
       <c r="B75" t="s">
-        <v>347</v>
+        <v>304</v>
       </c>
       <c r="C75" t="s">
         <v>64</v>
       </c>
       <c r="D75" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E75" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F75" t="s">
         <v>65</v>
       </c>
       <c r="G75" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H75" t="s">
-        <v>348</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AI Code Integrated to lastest Backend Code
</commit_message>
<xml_diff>
--- a/reference_data/plant_standards_cleaned.xlsx
+++ b/reference_data/plant_standards_cleaned.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\GreenEye_Backend\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\2025ESW\GreenEye_Backend\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF2773-3DE7-488B-A2D8-EC728A084DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42FFE59-B2C3-4720-8169-184E2EF562A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,9 +352,6 @@
     <t>20 ~ 60</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>22.0</t>
   </si>
   <si>
@@ -376,12 +373,6 @@
     <t>영산홍/철쭉 (Royal Azalea)</t>
   </si>
   <si>
-    <t>5 ~35</t>
-  </si>
-  <si>
-    <t>2200</t>
-  </si>
-  <si>
     <t>22 ~ 26</t>
   </si>
   <si>
@@ -559,9 +550,6 @@
     <t>25000 ~ 50000</t>
   </si>
   <si>
-    <t>10~30</t>
-  </si>
-  <si>
     <t>800 ~ 1500</t>
   </si>
   <si>
@@ -574,12 +562,6 @@
     <t>19 ~ 27</t>
   </si>
   <si>
-    <t>18~24</t>
-  </si>
-  <si>
-    <t>30~40</t>
-  </si>
-  <si>
     <t>400 ~ 1500</t>
   </si>
   <si>
@@ -589,12 +571,6 @@
     <t>에케베리아 (Echeveria)</t>
   </si>
   <si>
-    <t>16~24</t>
-  </si>
-  <si>
-    <t>20~40</t>
-  </si>
-  <si>
     <t>800 ~ 1600</t>
   </si>
   <si>
@@ -607,15 +583,6 @@
     <t>15 ~ 26</t>
   </si>
   <si>
-    <t>7000~15000</t>
-  </si>
-  <si>
-    <t>15~24</t>
-  </si>
-  <si>
-    <t>30~50</t>
-  </si>
-  <si>
     <t>1000 ~ 1800</t>
   </si>
   <si>
@@ -628,15 +595,6 @@
     <t>15 ~ 33</t>
   </si>
   <si>
-    <t>18000~30000</t>
-  </si>
-  <si>
-    <t>15~20</t>
-  </si>
-  <si>
-    <t>40~60</t>
-  </si>
-  <si>
     <t>1000 ~ 2000</t>
   </si>
   <si>
@@ -649,18 +607,6 @@
     <t>18 ~ 26</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>3600~12000</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>50~60</t>
-  </si>
-  <si>
     <t>44.0</t>
   </si>
   <si>
@@ -673,15 +619,6 @@
     <t>70 ~ 75</t>
   </si>
   <si>
-    <t>8000~15000</t>
-  </si>
-  <si>
-    <t>9~12</t>
-  </si>
-  <si>
-    <t>60~80</t>
-  </si>
-  <si>
     <t>45.0</t>
   </si>
   <si>
@@ -694,12 +631,6 @@
     <t>65 ~ 80</t>
   </si>
   <si>
-    <t>8~12</t>
-  </si>
-  <si>
-    <t>70~85</t>
-  </si>
-  <si>
     <t>1200 ~ 2500</t>
   </si>
   <si>
@@ -715,12 +646,6 @@
     <t>80 ~ 90</t>
   </si>
   <si>
-    <t>9~17</t>
-  </si>
-  <si>
-    <t>75~85</t>
-  </si>
-  <si>
     <t>1000 ~ 2200</t>
   </si>
   <si>
@@ -733,12 +658,6 @@
     <t>5 ~ 17</t>
   </si>
   <si>
-    <t>10000~20000</t>
-  </si>
-  <si>
-    <t>10~16</t>
-  </si>
-  <si>
     <t>1200 ~ 2000</t>
   </si>
   <si>
@@ -748,12 +667,6 @@
     <t>글라디올러스 (Gladiolus)</t>
   </si>
   <si>
-    <t>25000~40000</t>
-  </si>
-  <si>
-    <t>65~80</t>
-  </si>
-  <si>
     <t>1400 ~ 2400</t>
   </si>
   <si>
@@ -763,12 +676,6 @@
     <t>아마릴리스 (Amaryllis)</t>
   </si>
   <si>
-    <t>10000~25000</t>
-  </si>
-  <si>
-    <t>50~70</t>
-  </si>
-  <si>
     <t>50.0</t>
   </si>
   <si>
@@ -778,12 +685,6 @@
     <t>4 ~ 15</t>
   </si>
   <si>
-    <t>8000~20000</t>
-  </si>
-  <si>
-    <t>5~12</t>
-  </si>
-  <si>
     <t>51.0</t>
   </si>
   <si>
@@ -805,12 +706,6 @@
     <t>65 ~ 75</t>
   </si>
   <si>
-    <t>15000~30000</t>
-  </si>
-  <si>
-    <t>17~24</t>
-  </si>
-  <si>
     <t>1800 ~ 2500</t>
   </si>
   <si>
@@ -826,9 +721,6 @@
     <t>70 ~ 90</t>
   </si>
   <si>
-    <t>15000~27000</t>
-  </si>
-  <si>
     <t>54.0</t>
   </si>
   <si>
@@ -841,9 +733,6 @@
     <t>70 ~ 80</t>
   </si>
   <si>
-    <t>9~18</t>
-  </si>
-  <si>
     <t>1400 ~ 2500</t>
   </si>
   <si>
@@ -856,12 +745,6 @@
     <t>65 ~ 85</t>
   </si>
   <si>
-    <t>16~22</t>
-  </si>
-  <si>
-    <t>60~75</t>
-  </si>
-  <si>
     <t>2000 ~ 3500</t>
   </si>
   <si>
@@ -874,12 +757,6 @@
     <t>17 ~ 34</t>
   </si>
   <si>
-    <t>25000~100000</t>
-  </si>
-  <si>
-    <t>12~20</t>
-  </si>
-  <si>
     <t>500 ~ 2000</t>
   </si>
   <si>
@@ -895,202 +772,362 @@
     <t>810 ~ 2150</t>
   </si>
   <si>
+    <t>58.0</t>
+  </si>
+  <si>
+    <t>아글라오네마 (Aglaonema)</t>
+  </si>
+  <si>
+    <t>45 ~ 60</t>
+  </si>
+  <si>
+    <t>270 ~ 2150</t>
+  </si>
+  <si>
+    <t>59.0</t>
+  </si>
+  <si>
+    <t>디펜바키아 (Dieffenbachia)</t>
+  </si>
+  <si>
+    <t>1600 ~ 2700</t>
+  </si>
+  <si>
+    <t>30 ~ 40</t>
+  </si>
+  <si>
+    <t>1200 ~ 2200</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>몬스테라 (Monstera)</t>
+  </si>
+  <si>
+    <t>800 ~ 10000</t>
+  </si>
+  <si>
+    <t>28 ~ 38</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>산세베리아 (Sansevieria)</t>
+  </si>
+  <si>
+    <t>21 ~ 25</t>
+  </si>
+  <si>
+    <t>270 ~ 4300</t>
+  </si>
+  <si>
+    <t>22 ~ 25</t>
+  </si>
+  <si>
+    <t>12 ~ 22</t>
+  </si>
+  <si>
+    <t>500 ~ 1200</t>
+  </si>
+  <si>
+    <t>62.0</t>
+  </si>
+  <si>
+    <t>테이블야자 (Parlor palm)</t>
+  </si>
+  <si>
+    <t>20 ~ 27</t>
+  </si>
+  <si>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>페페로미아 (Peperomia)</t>
+  </si>
+  <si>
+    <t>25 ~ 35</t>
+  </si>
+  <si>
+    <t>800 ~ 1800</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>벵갈고무나무 (Ficus elastica)</t>
+  </si>
+  <si>
+    <t>810 ~ 4300</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>싱고니움 (Syngonium)</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>칼라디움 (Caladium)</t>
+  </si>
+  <si>
+    <t>35 ~ 45</t>
+  </si>
+  <si>
+    <t>67.0</t>
+  </si>
+  <si>
+    <t>바질 (Basil)</t>
+  </si>
+  <si>
+    <t>20000 ~ 100000</t>
+  </si>
+  <si>
+    <t>30 ~ 45</t>
+  </si>
+  <si>
+    <t>1300 ~ 2000</t>
+  </si>
+  <si>
+    <t>68.0</t>
+  </si>
+  <si>
+    <t>로즈마리 (Rosemary)</t>
+  </si>
+  <si>
+    <t>40 ~ 50</t>
+  </si>
+  <si>
+    <t>69.0</t>
+  </si>
+  <si>
+    <t>타임 / 벼룩이자리 (Thyme)</t>
+  </si>
+  <si>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>오레가노 (Oregano)</t>
+  </si>
+  <si>
+    <t>71.0</t>
+  </si>
+  <si>
+    <t>민트 / 배초향 (Korean Mint)</t>
+  </si>
+  <si>
+    <t>72.0</t>
+  </si>
+  <si>
+    <t>73.0</t>
+  </si>
+  <si>
+    <t>카모마일 / 카밀레 (Chamomile)</t>
+  </si>
+  <si>
+    <t>1000 ~ 1600</t>
+  </si>
+  <si>
+    <t>74.0</t>
+  </si>
+  <si>
+    <t>안개꽃 (Gypsophila)</t>
+  </si>
+  <si>
+    <t>1250 ~ 2000</t>
+  </si>
+  <si>
+    <t>1800 ~ 2200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500 ~ 2500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40 ~ 60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 ~ 25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 ~ 35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 ~ 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8 ~ 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 ~ 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 ~ 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 ~ 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7000 ~ 15000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18000 ~ 30000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3600 ~ 12000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000 ~ 15000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000 ~ 20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25000 ~ 40000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000 ~ 25000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000 ~ 20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15000 ~ 30000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15000 ~ 27000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25000 ~ 100000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 ~ 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16 ~ 22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17 ~ 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9 ~ 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 ~ 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 ~ 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 ~ 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 ~ 60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 ~ 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70 ~ 85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75 ~ 85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65 ~ 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 ~ 70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 ~ 75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>25 ~ 30</t>
-  </si>
-  <si>
-    <t>58.0</t>
-  </si>
-  <si>
-    <t>아글라오네마 (Aglaonema)</t>
-  </si>
-  <si>
-    <t>45 ~ 60</t>
-  </si>
-  <si>
-    <t>270 ~ 2150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>30 ~ 38</t>
-  </si>
-  <si>
-    <t>59.0</t>
-  </si>
-  <si>
-    <t>디펜바키아 (Dieffenbachia)</t>
-  </si>
-  <si>
-    <t>1600 ~ 2700</t>
-  </si>
-  <si>
-    <t>30 ~ 40</t>
-  </si>
-  <si>
-    <t>1200 ~ 2200</t>
-  </si>
-  <si>
-    <t>60.0</t>
-  </si>
-  <si>
-    <t>몬스테라 (Monstera)</t>
-  </si>
-  <si>
-    <t>800 ~ 10000</t>
-  </si>
-  <si>
-    <t>28 ~ 38</t>
-  </si>
-  <si>
-    <t>61.0</t>
-  </si>
-  <si>
-    <t>산세베리아 (Sansevieria)</t>
-  </si>
-  <si>
-    <t>21 ~ 25</t>
-  </si>
-  <si>
-    <t>270 ~ 4300</t>
-  </si>
-  <si>
-    <t>22 ~ 25</t>
-  </si>
-  <si>
-    <t>12 ~ 22</t>
-  </si>
-  <si>
-    <t>500 ~ 1200</t>
-  </si>
-  <si>
-    <t>62.0</t>
-  </si>
-  <si>
-    <t>테이블야자 (Parlor palm)</t>
-  </si>
-  <si>
-    <t>20 ~ 27</t>
-  </si>
-  <si>
-    <t>63.0</t>
-  </si>
-  <si>
-    <t>페페로미아 (Peperomia)</t>
-  </si>
-  <si>
-    <t>25 ~ 35</t>
-  </si>
-  <si>
-    <t>800 ~ 1800</t>
-  </si>
-  <si>
-    <t>64.0</t>
-  </si>
-  <si>
-    <t>벵갈고무나무 (Ficus elastica)</t>
-  </si>
-  <si>
-    <t>810 ~ 4300</t>
-  </si>
-  <si>
-    <t>65.0</t>
-  </si>
-  <si>
-    <t>싱고니움 (Syngonium)</t>
-  </si>
-  <si>
-    <t>66.0</t>
-  </si>
-  <si>
-    <t>칼라디움 (Caladium)</t>
-  </si>
-  <si>
-    <t>35 ~ 45</t>
-  </si>
-  <si>
-    <t>67.0</t>
-  </si>
-  <si>
-    <t>바질 (Basil)</t>
-  </si>
-  <si>
-    <t>20000 ~ 100000</t>
-  </si>
-  <si>
-    <t>30 ~ 45</t>
-  </si>
-  <si>
-    <t>1300 ~ 2000</t>
-  </si>
-  <si>
-    <t>68.0</t>
-  </si>
-  <si>
-    <t>로즈마리 (Rosemary)</t>
-  </si>
-  <si>
-    <t>40 ~ 50</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
-    <t>타임 / 벼룩이자리 (Thyme)</t>
-  </si>
-  <si>
-    <t>70.0</t>
-  </si>
-  <si>
-    <t>오레가노 (Oregano)</t>
-  </si>
-  <si>
-    <t>71.0</t>
-  </si>
-  <si>
-    <t>민트 / 배초향 (Korean Mint)</t>
-  </si>
-  <si>
-    <t>72.0</t>
-  </si>
-  <si>
-    <t>73.0</t>
-  </si>
-  <si>
-    <t>카모마일 / 카밀레 (Chamomile)</t>
-  </si>
-  <si>
-    <t>1000 ~ 1600</t>
-  </si>
-  <si>
-    <t>74.0</t>
-  </si>
-  <si>
-    <t>안개꽃 (Gypsophila)</t>
-  </si>
-  <si>
-    <t>1250 ~ 2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>환경온도(°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>환경습도(%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>환경광도(lux)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>토양온도(°C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>토양수분(%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>토양전도도(uS/cm)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1465,10 +1502,19 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <cols>
+    <col min="2" max="2" width="28.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -2039,15 +2085,15 @@
         <v>109</v>
       </c>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
         <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
       </c>
       <c r="C23" t="s">
         <v>106</v>
@@ -2056,50 +2102,50 @@
         <v>16</v>
       </c>
       <c r="E23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" t="s">
         <v>113</v>
-      </c>
-      <c r="F23" t="s">
-        <v>114</v>
       </c>
       <c r="G23" t="s">
         <v>108</v>
       </c>
       <c r="H23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
         <v>116</v>
       </c>
-      <c r="B24" t="s">
-        <v>117</v>
-      </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>311</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
+        <v>307</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" t="s">
         <v>119</v>
-      </c>
-      <c r="F24" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
         <v>64</v>
@@ -2108,10 +2154,10 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G25" t="s">
         <v>8</v>
@@ -2122,45 +2168,45 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
         <v>108</v>
       </c>
       <c r="H26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -2174,22 +2220,22 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" t="s">
         <v>16</v>
@@ -2200,51 +2246,51 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H30" t="s">
         <v>61</v>
@@ -2252,22 +2298,22 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31" t="s">
         <v>16</v>
@@ -2278,19 +2324,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F32" t="s">
         <v>108</v>
@@ -2304,10 +2350,10 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
         <v>36</v>
@@ -2316,85 +2362,85 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F33" t="s">
         <v>36</v>
       </c>
       <c r="G33" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G34" t="s">
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G35" t="s">
         <v>94</v>
       </c>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F36" t="s">
         <v>25</v>
@@ -2403,30 +2449,30 @@
         <v>94</v>
       </c>
       <c r="H36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H37" t="s">
         <v>86</v>
@@ -2434,10 +2480,10 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
@@ -2449,307 +2495,307 @@
         <v>99</v>
       </c>
       <c r="F38" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G38" t="s">
         <v>94</v>
       </c>
       <c r="H38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G39" t="s">
-        <v>179</v>
+        <v>335</v>
       </c>
       <c r="H39" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F40" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="G40" t="s">
-        <v>185</v>
+        <v>336</v>
       </c>
       <c r="H40" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C41" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F41" t="s">
-        <v>189</v>
+        <v>319</v>
       </c>
       <c r="G41" t="s">
-        <v>190</v>
+        <v>337</v>
       </c>
       <c r="H41" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>195</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="G42" t="s">
-        <v>197</v>
+        <v>338</v>
       </c>
       <c r="H42" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B43" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D43" t="s">
         <v>16</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
+        <v>321</v>
       </c>
       <c r="F43" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="G43" t="s">
-        <v>204</v>
+        <v>309</v>
       </c>
       <c r="H43" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B44" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>209</v>
+        <v>309</v>
       </c>
       <c r="E44" t="s">
-        <v>210</v>
+        <v>322</v>
       </c>
       <c r="F44" t="s">
-        <v>211</v>
+        <v>310</v>
       </c>
       <c r="G44" t="s">
-        <v>212</v>
+        <v>339</v>
       </c>
       <c r="H44" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C45" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="D45" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="F45" t="s">
-        <v>218</v>
+        <v>312</v>
       </c>
       <c r="G45" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H45" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="C46" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="E46" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="F46" t="s">
-        <v>224</v>
+        <v>313</v>
       </c>
       <c r="G46" t="s">
-        <v>225</v>
+        <v>341</v>
       </c>
       <c r="H46" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="B47" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="C47" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="E47" t="s">
-        <v>217</v>
+        <v>323</v>
       </c>
       <c r="F47" t="s">
-        <v>231</v>
+        <v>314</v>
       </c>
       <c r="G47" t="s">
-        <v>232</v>
+        <v>342</v>
       </c>
       <c r="H47" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="B48" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="C48" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E48" t="s">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="F48" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="G48" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H48" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>308</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E49" t="s">
-        <v>242</v>
+        <v>325</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="G49" t="s">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="H49" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
         <v>64</v>
@@ -2758,258 +2804,258 @@
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>247</v>
+        <v>326</v>
       </c>
       <c r="F50" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="G50" t="s">
-        <v>248</v>
+        <v>345</v>
       </c>
       <c r="H50" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="C51" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="D51" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="E51" t="s">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="F51" t="s">
-        <v>253</v>
+        <v>317</v>
       </c>
       <c r="G51" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H51" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="C52" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D52" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="E52" t="s">
-        <v>242</v>
+        <v>325</v>
       </c>
       <c r="F52" t="s">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="G52" t="s">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="H52" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="E53" t="s">
-        <v>261</v>
+        <v>328</v>
       </c>
       <c r="F53" t="s">
-        <v>262</v>
+        <v>333</v>
       </c>
       <c r="G53" t="s">
-        <v>225</v>
+        <v>341</v>
       </c>
       <c r="H53" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="C54" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="D54" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="E54" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
       <c r="F54" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="G54" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H54" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="C55" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D55" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="E55" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
       <c r="F55" t="s">
-        <v>273</v>
+        <v>334</v>
       </c>
       <c r="G55" t="s">
-        <v>243</v>
+        <v>344</v>
       </c>
       <c r="H55" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
       <c r="B56" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
       <c r="C56" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D56" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
       <c r="E56" t="s">
-        <v>268</v>
+        <v>329</v>
       </c>
       <c r="F56" t="s">
-        <v>278</v>
+        <v>332</v>
       </c>
       <c r="G56" t="s">
-        <v>279</v>
+        <v>346</v>
       </c>
       <c r="H56" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>281</v>
+        <v>242</v>
       </c>
       <c r="B57" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="C57" t="s">
-        <v>283</v>
+        <v>244</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>284</v>
+        <v>330</v>
       </c>
       <c r="F57" t="s">
-        <v>285</v>
+        <v>331</v>
       </c>
       <c r="G57" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="H57" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="B58" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
       <c r="C58" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="D58" t="s">
         <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="F58" t="s">
         <v>36</v>
       </c>
       <c r="G58" t="s">
-        <v>291</v>
+        <v>347</v>
       </c>
       <c r="H58" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>292</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
       <c r="C59" t="s">
         <v>108</v>
       </c>
       <c r="D59" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="E59" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="F59" t="s">
         <v>108</v>
       </c>
       <c r="G59" t="s">
-        <v>296</v>
+        <v>348</v>
       </c>
       <c r="H59" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B60" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
@@ -3018,24 +3064,24 @@
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="F60" t="s">
         <v>108</v>
       </c>
       <c r="G60" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H60" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C61" t="s">
         <v>25</v>
@@ -3044,76 +3090,76 @@
         <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>304</v>
+        <v>261</v>
       </c>
       <c r="F61" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G61" t="s">
-        <v>305</v>
+        <v>262</v>
       </c>
       <c r="H61" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="C62" t="s">
-        <v>308</v>
+        <v>265</v>
       </c>
       <c r="D62" t="s">
         <v>16</v>
       </c>
       <c r="E62" t="s">
-        <v>309</v>
+        <v>266</v>
       </c>
       <c r="F62" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G62" t="s">
-        <v>311</v>
+        <v>268</v>
       </c>
       <c r="H62" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="B63" t="s">
-        <v>314</v>
+        <v>271</v>
       </c>
       <c r="C63" t="s">
-        <v>315</v>
+        <v>272</v>
       </c>
       <c r="D63" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="E63" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="F63" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G63" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H63" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>316</v>
+        <v>273</v>
       </c>
       <c r="B64" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="C64" t="s">
         <v>36</v>
@@ -3122,180 +3168,180 @@
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="F64" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G64" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H64" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>320</v>
+        <v>277</v>
       </c>
       <c r="B65" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="C65" t="s">
         <v>36</v>
       </c>
       <c r="D65" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="E65" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="F65" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G65" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H65" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>323</v>
+        <v>280</v>
       </c>
       <c r="B66" t="s">
-        <v>324</v>
+        <v>281</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="F66" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="G66" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H66" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>325</v>
+        <v>282</v>
       </c>
       <c r="B67" t="s">
-        <v>326</v>
+        <v>283</v>
       </c>
       <c r="C67" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D67" t="s">
         <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="F67" t="s">
         <v>48</v>
       </c>
       <c r="G67" t="s">
-        <v>327</v>
+        <v>284</v>
       </c>
       <c r="H67" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="B68" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F68" t="s">
         <v>65</v>
       </c>
       <c r="G68" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="H68" t="s">
-        <v>332</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>333</v>
+        <v>290</v>
       </c>
       <c r="B69" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="C69" t="s">
         <v>15</v>
       </c>
       <c r="D69" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E69" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F69" t="s">
         <v>65</v>
       </c>
       <c r="G69" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H69" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="B70" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="C70" t="s">
         <v>15</v>
       </c>
       <c r="D70" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E70" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F70" t="s">
         <v>65</v>
       </c>
       <c r="G70" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H70" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
       <c r="B71" t="s">
-        <v>339</v>
+        <v>296</v>
       </c>
       <c r="C71" t="s">
         <v>15</v>
@@ -3304,47 +3350,47 @@
         <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F71" t="s">
         <v>65</v>
       </c>
       <c r="G71" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H71" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>340</v>
+        <v>297</v>
       </c>
       <c r="B72" t="s">
-        <v>341</v>
+        <v>298</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F72" t="s">
         <v>65</v>
       </c>
       <c r="G72" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H72" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
@@ -3356,68 +3402,68 @@
         <v>19</v>
       </c>
       <c r="E73" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F73" t="s">
         <v>65</v>
       </c>
       <c r="G73" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H73" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>343</v>
+        <v>300</v>
       </c>
       <c r="B74" t="s">
-        <v>344</v>
+        <v>301</v>
       </c>
       <c r="C74" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="D74" t="s">
         <v>5</v>
       </c>
       <c r="E74" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F74" t="s">
         <v>65</v>
       </c>
       <c r="G74" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H74" t="s">
-        <v>345</v>
+        <v>302</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>346</v>
+        <v>303</v>
       </c>
       <c r="B75" t="s">
-        <v>347</v>
+        <v>304</v>
       </c>
       <c r="C75" t="s">
         <v>64</v>
       </c>
       <c r="D75" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="E75" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="F75" t="s">
         <v>65</v>
       </c>
       <c r="G75" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="H75" t="s">
-        <v>348</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>